<commit_message>
Emptying the charts in the word documents
</commit_message>
<xml_diff>
--- a/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
+++ b/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Time</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Plasma Renin</t>
+  </si>
+  <si>
+    <t>***QCP has an error just before the hour is complete giving incorrect values</t>
   </si>
 </sst>
 </file>
@@ -73,12 +76,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -141,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -161,6 +170,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,7 +477,7 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -486,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -504,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45.75" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -522,7 +533,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="45.75" thickBot="1">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -540,7 +551,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="45.75" thickBot="1">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -558,7 +569,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -576,7 +587,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="30.75" thickBot="1">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -594,7 +605,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="30.75" thickBot="1">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -612,7 +623,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="30.75" thickBot="1">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -630,7 +641,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="30.75" thickBot="1">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -648,7 +659,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="30.75" thickBot="1">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -665,6 +676,17 @@
         <v>3.5</v>
       </c>
       <c r="F11" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
+      <c r="A13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixing my notes in the QCP guide
</commit_message>
<xml_diff>
--- a/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
+++ b/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
@@ -164,14 +164,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +478,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
@@ -498,7 +498,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -678,15 +678,15 @@
       <c r="F11" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Adding Lab 17 HumMod data
</commit_message>
<xml_diff>
--- a/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
+++ b/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>mL/min</t>
+  </si>
+  <si>
+    <t>bpm</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>At roughly 45 minutes, the patient dies, recording data at V-fib</t>
   </si>
 </sst>
 </file>
@@ -93,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,39 +138,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -153,27 +147,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,241 +475,510 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="4">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="4">
         <v>10</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="4">
         <v>20</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="4">
         <v>30</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="4">
+        <v>0</v>
+      </c>
+      <c r="M1" s="4">
+        <v>10</v>
+      </c>
+      <c r="N1" s="4">
+        <v>20</v>
+      </c>
+      <c r="O1" s="4">
+        <v>30</v>
+      </c>
+      <c r="P1" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="45.75" thickBot="1">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="7">
         <v>552</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>592</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="7">
         <v>617</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="7">
         <v>634</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="7">
+        <v>545</v>
+      </c>
+      <c r="M3" s="7">
+        <v>591</v>
+      </c>
+      <c r="N3" s="7">
+        <v>619</v>
+      </c>
+      <c r="O3" s="7">
+        <v>640</v>
+      </c>
+      <c r="P3" s="7">
+        <v>666</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="45.75" thickBot="1">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="7">
         <v>97</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="7">
         <v>84</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>70</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="7">
         <v>53</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="7">
+        <v>96.6</v>
+      </c>
+      <c r="M4" s="7">
+        <v>93.3</v>
+      </c>
+      <c r="N4" s="7">
+        <v>86.5</v>
+      </c>
+      <c r="O4" s="7">
+        <v>75</v>
+      </c>
+      <c r="P4" s="7">
+        <v>49.5</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="45.75" thickBot="1">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="7">
         <v>5346</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="7">
         <v>4564</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="7">
         <v>3634</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>2600</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="7">
+        <v>5468</v>
+      </c>
+      <c r="M5" s="7">
+        <v>5545</v>
+      </c>
+      <c r="N5" s="7">
+        <v>5206</v>
+      </c>
+      <c r="O5" s="7">
+        <v>4411</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="7">
         <v>72</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="7">
         <v>77</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>84</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="7">
         <v>87</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="G6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="7">
+        <v>72</v>
+      </c>
+      <c r="M6" s="7">
+        <v>75</v>
+      </c>
+      <c r="N6" s="7">
+        <v>81</v>
+      </c>
+      <c r="O6" s="7">
+        <v>89</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="7">
         <v>75</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="7">
         <v>59</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="7">
         <v>43</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="7">
+        <v>76</v>
+      </c>
+      <c r="M7" s="7">
+        <v>74</v>
+      </c>
+      <c r="N7" s="7">
+        <v>64</v>
+      </c>
+      <c r="O7" s="7">
+        <v>50</v>
+      </c>
+      <c r="P7" s="7">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="7">
         <v>124</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="7">
         <v>98</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="7">
         <v>74</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="7">
         <v>53</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A9" s="3" t="s">
+      <c r="G8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="M8" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="N8" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="O8" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="P8" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="7">
         <v>3.4</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="7">
         <v>3.8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="7">
         <v>6.4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A10" s="3" t="s">
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="7">
+        <v>126.7</v>
+      </c>
+      <c r="M9" s="7">
+        <v>115</v>
+      </c>
+      <c r="N9" s="7">
+        <v>94</v>
+      </c>
+      <c r="O9" s="7">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="P9" s="7">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="7">
         <v>1.5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7">
         <v>1.7</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="7">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A11" s="3" t="s">
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="N10" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="O10" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P10" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30.75" thickBot="1">
+      <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="7">
         <v>2</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="7">
         <v>2.1</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="7">
         <v>2.6</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="7">
         <v>3.7</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="5" t="s">
+      <c r="G11" s="5"/>
+      <c r="K11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M11" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N11" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="O11" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="P11" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="K13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="K13:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding percentage data to Lab 17
</commit_message>
<xml_diff>
--- a/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
+++ b/17_pericardial_hemorrhage/pericardial_hemorrhage_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="24">
   <si>
     <t>Time</t>
   </si>
@@ -85,13 +85,16 @@
   </si>
   <si>
     <t>At roughly 45 minutes, the patient dies, recording data at V-fib</t>
+  </si>
+  <si>
+    <t>Diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +107,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -144,10 +154,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -164,17 +175,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -464,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,8 +525,8 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
@@ -497,7 +547,7 @@
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="3">
@@ -518,9 +568,30 @@
       <c r="Q1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="U1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="3">
+        <v>0</v>
+      </c>
+      <c r="W1" s="3">
+        <v>10</v>
+      </c>
+      <c r="X1" s="3">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1">
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -539,7 +610,7 @@
       <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="8"/>
       <c r="L2" s="3" t="s">
         <v>1</v>
       </c>
@@ -558,8 +629,27 @@
       <c r="Q2" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="U2" s="8"/>
+      <c r="V2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="45.75" thickBot="1">
+    <row r="3" spans="1:27" ht="45.75" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -602,8 +692,33 @@
       <c r="Q3" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="U3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="11">
+        <f>ABS((B3-L3)/B3)</f>
+        <v>1.2681159420289856E-2</v>
+      </c>
+      <c r="W3" s="11">
+        <f t="shared" ref="W3:W11" si="0">ABS((C3-M3)/C3)</f>
+        <v>1.6891891891891893E-3</v>
+      </c>
+      <c r="X3" s="11">
+        <f t="shared" ref="X3:X11" si="1">ABS((D3-N3)/D3)</f>
+        <v>3.2414910858995136E-3</v>
+      </c>
+      <c r="Y3" s="11">
+        <f t="shared" ref="Y3:Y11" si="2">ABS((E3-O3)/E3)</f>
+        <v>9.4637223974763408E-3</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="45.75" thickBot="1">
+    <row r="4" spans="1:27" ht="45.75" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -646,8 +761,33 @@
       <c r="Q4" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="U4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="11">
+        <f t="shared" ref="V4:V11" si="3">ABS((B4-L4)/B4)</f>
+        <v>4.1237113402062438E-3</v>
+      </c>
+      <c r="W4" s="11">
+        <f t="shared" si="0"/>
+        <v>0.11071428571428568</v>
+      </c>
+      <c r="X4" s="11">
+        <f t="shared" si="1"/>
+        <v>0.23571428571428571</v>
+      </c>
+      <c r="Y4" s="11">
+        <f t="shared" si="2"/>
+        <v>0.41509433962264153</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="45.75" thickBot="1">
+    <row r="5" spans="1:27" ht="45.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -690,8 +830,33 @@
       <c r="Q5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="U5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="11">
+        <f t="shared" si="3"/>
+        <v>2.2820800598578377E-2</v>
+      </c>
+      <c r="W5" s="11">
+        <f t="shared" si="0"/>
+        <v>0.214943032427695</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="1"/>
+        <v>0.43258117776554761</v>
+      </c>
+      <c r="Y5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.69653846153846155</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="30.75" thickBot="1">
+    <row r="6" spans="1:27" ht="30.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -734,8 +899,33 @@
       <c r="Q6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="U6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="11">
+        <f t="shared" si="0"/>
+        <v>2.5974025974025976E-2</v>
+      </c>
+      <c r="X6" s="11">
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="Y6" s="11">
+        <f t="shared" si="2"/>
+        <v>2.2988505747126436E-2</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="30.75" thickBot="1">
+    <row r="7" spans="1:27" ht="30.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -778,8 +968,33 @@
       <c r="Q7" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="U7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="V7" s="11">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="W7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.25423728813559321</v>
+      </c>
+      <c r="X7" s="11">
+        <f t="shared" si="1"/>
+        <v>0.48837209302325579</v>
+      </c>
+      <c r="Y7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="30.75" thickBot="1">
+    <row r="8" spans="1:27" ht="30.75" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -822,8 +1037,33 @@
       <c r="Q8" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="U8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V8" s="11">
+        <f t="shared" si="3"/>
+        <v>2.1774193548387121E-2</v>
+      </c>
+      <c r="W8" s="11">
+        <f t="shared" si="0"/>
+        <v>0.17346938775510204</v>
+      </c>
+      <c r="X8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.27027027027027029</v>
+      </c>
+      <c r="Y8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.28490566037735837</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="30.75" thickBot="1">
+    <row r="9" spans="1:27" ht="30.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -866,8 +1106,33 @@
       <c r="Q9" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="U9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" s="11">
+        <f t="shared" si="3"/>
+        <v>0.52941176470588247</v>
+      </c>
+      <c r="W9" s="11">
+        <f t="shared" si="0"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="X9" s="11">
+        <f t="shared" si="1"/>
+        <v>0.11999999999999993</v>
+      </c>
+      <c r="Y9" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10937500000000003</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="30.75" thickBot="1">
+    <row r="10" spans="1:27" ht="30.75" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -910,8 +1175,33 @@
       <c r="Q10" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="U10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="11">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764629E-2</v>
+      </c>
+      <c r="X10" s="11">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="Y10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="30.75" thickBot="1">
+    <row r="11" spans="1:27" ht="30.75" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -950,8 +1240,31 @@
         <v>7.5</v>
       </c>
       <c r="Q11" s="4"/>
+      <c r="U11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="11">
+        <f t="shared" si="3"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="W11" s="11">
+        <f t="shared" si="0"/>
+        <v>9.5238095238095108E-2</v>
+      </c>
+      <c r="X11" s="11">
+        <f t="shared" si="1"/>
+        <v>7.6923076923076816E-2</v>
+      </c>
+      <c r="Y11" s="11">
+        <f t="shared" si="2"/>
+        <v>0.16216216216216206</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA11" s="4"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75">
+    <row r="13" spans="1:27" ht="15.75">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -961,18 +1274,18 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:27" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:27" ht="15.75" thickBot="1">
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -980,11 +1293,21 @@
       <c r="N15" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="K13:Q13"/>
+    <mergeCell ref="U1:U2"/>
   </mergeCells>
+  <conditionalFormatting sqref="V3:Y11">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>